<commit_message>
Auto-committed on 2023/08/30 週三 11:43:40.75
</commit_message>
<xml_diff>
--- a/Program/Other/LM053_底稿_法務分配款明細表_內部控管.xlsx
+++ b/Program/Other/LM053_底稿_法務分配款明細表_內部控管.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77E6163-1919-4BEC-BF67-B11D449B65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484"/>
+    <workbookView xWindow="800" yWindow="3310" windowWidth="18380" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="法務分配表" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">法務分配表!$A$2:$L$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">法務分配表!$A$1:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">法務分配表!$A$2:$N$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">法務分配表!$A$1:$N$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">法務分配表!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>地區</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -46,42 +47,46 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>不足額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>入帳日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>分配表日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>損失率 %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>法務人員</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>額度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>債權金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>拍定金額</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>不足額</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>入帳日</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>分配表日期</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>損失率 %</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>法務人員</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>額度</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
+    <t>領取分配金額</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -89,7 +94,7 @@
     <numFmt numFmtId="177" formatCode="[$-404]e/m/d;@"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -106,13 +111,6 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="1"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
@@ -158,30 +156,12 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -231,108 +211,84 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -353,9 +309,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,9 +349,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,7 +386,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,7 +421,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -638,204 +594,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16" style="8" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" style="10" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" style="10" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="3" style="17" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="10.6328125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="6.90625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="14" customWidth="1"/>
+    <col min="6" max="10" width="16" style="22" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="23" customWidth="1"/>
+    <col min="12" max="12" width="6.90625" style="24" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.6328125" style="25" customWidth="1"/>
+    <col min="15" max="15" width="3" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="8.90625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="15" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="17"/>
-    </row>
-    <row r="2" spans="1:13" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A2" s="21" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="21" customHeight="1">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="26" t="s">
+      <c r="M2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="21" t="s">
+      <c r="N2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="1"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="12"/>
+    <row r="3" spans="1:15">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L10"/>
+  <autoFilter ref="A2:N10" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.27559055118110237" right="0.23622047244094491" top="0.59055118110236227" bottom="0.55118110236220474" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="73" fitToHeight="10" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>